<commit_message>
Updated usage section to include information about the Excel sheet
</commit_message>
<xml_diff>
--- a/testlist.xlsx
+++ b/testlist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andymcgallian/Desktop/M-TEMP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08CEB6D9-0E1E-7442-AEF9-BC5AC195279D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA375AA-BE5F-EE40-963B-9B9A5B042621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1040" yWindow="560" windowWidth="22920" windowHeight="13160" xr2:uid="{5E4CCF26-D717-4450-9E39-3C5B3D233C01}"/>
   </bookViews>
@@ -38,60 +38,27 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
-    <t>date</t>
-  </si>
-  <si>
     <t>USB-TEMP (Device 0) - Analog - 9-16-2024 2-09-36.6 PM.csv'</t>
   </si>
   <si>
-    <t>testing route</t>
-  </si>
-  <si>
     <t>indoor  QC pre-check</t>
   </si>
   <si>
-    <t>cart</t>
-  </si>
-  <si>
-    <t>set up</t>
-  </si>
-  <si>
     <t>4-wire</t>
   </si>
   <si>
-    <t>test num</t>
-  </si>
-  <si>
-    <t>folder</t>
-  </si>
-  <si>
-    <t>temperature data</t>
-  </si>
-  <si>
     <t>QA Testing 091624/Cart 1 Indoor Data/'</t>
   </si>
   <si>
-    <t>IR/RH data</t>
-  </si>
-  <si>
     <t>USB-1208FS-Plus (Device 1) - Analog - 9-16-2024 2-09-37.1 PM.csv'</t>
   </si>
   <si>
-    <t>GPS data</t>
-  </si>
-  <si>
     <t>None'</t>
   </si>
   <si>
     <t>Cart 1 Temp'</t>
   </si>
   <si>
-    <t>IR Configuration</t>
-  </si>
-  <si>
-    <t>Temp Configuration</t>
-  </si>
-  <si>
     <t>Cart 1 IR'</t>
   </si>
   <si>
@@ -105,6 +72,39 @@
   </si>
   <si>
     <t>outdoor QC</t>
+  </si>
+  <si>
+    <t>Test Number</t>
+  </si>
+  <si>
+    <t>Test Folder</t>
+  </si>
+  <si>
+    <t>Temperature Data</t>
+  </si>
+  <si>
+    <t>IR/RH Data</t>
+  </si>
+  <si>
+    <t>GPS Data</t>
+  </si>
+  <si>
+    <t>Test Date</t>
+  </si>
+  <si>
+    <t>Testing Route</t>
+  </si>
+  <si>
+    <t>Cart</t>
+  </si>
+  <si>
+    <t>Set Up</t>
+  </si>
+  <si>
+    <t>Temperature Configuration</t>
+  </si>
+  <si>
+    <t>IR/RH Configuration</t>
   </si>
 </sst>
 </file>
@@ -481,7 +481,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -496,37 +496,37 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F1" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="G1" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="H1" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="I1" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="J1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="K1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -534,34 +534,34 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="F2" s="2">
         <v>45551</v>
       </c>
       <c r="G2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
       <c r="I2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="K2" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -569,34 +569,34 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="F3" s="2">
         <v>45551</v>
       </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
       <c r="I3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="K3" s="1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Checkpoint for the evening
</commit_message>
<xml_diff>
--- a/testlist.xlsx
+++ b/testlist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andymcgallian/Desktop/M-TEMP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA375AA-BE5F-EE40-963B-9B9A5B042621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB0CA8F-E993-9A41-98A2-45E8E2C78A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="560" windowWidth="22920" windowHeight="13160" xr2:uid="{5E4CCF26-D717-4450-9E39-3C5B3D233C01}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16360" xr2:uid="{5E4CCF26-D717-4450-9E39-3C5B3D233C01}"/>
   </bookViews>
   <sheets>
     <sheet name="tests" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
-  <si>
-    <t>USB-TEMP (Device 0) - Analog - 9-16-2024 2-09-36.6 PM.csv'</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
   <si>
     <t>indoor  QC pre-check</t>
   </si>
@@ -47,30 +44,6 @@
     <t>4-wire</t>
   </si>
   <si>
-    <t>QA Testing 091624/Cart 1 Indoor Data/'</t>
-  </si>
-  <si>
-    <t>USB-1208FS-Plus (Device 1) - Analog - 9-16-2024 2-09-37.1 PM.csv'</t>
-  </si>
-  <si>
-    <t>None'</t>
-  </si>
-  <si>
-    <t>Cart 1 Temp'</t>
-  </si>
-  <si>
-    <t>Cart 1 IR'</t>
-  </si>
-  <si>
-    <t>QA Testing 091624/Cart 1 Outdoor Data/'</t>
-  </si>
-  <si>
-    <t>USB-TEMP (Device 0) - Analog - 9-16-2024 1-09-41.2 PM.csv'</t>
-  </si>
-  <si>
-    <t>USB-1208FS-Plus (Device 1) - Analog - 9-16-2024 1-09-41.7 PM.csv'</t>
-  </si>
-  <si>
     <t>outdoor QC</t>
   </si>
   <si>
@@ -105,6 +78,63 @@
   </si>
   <si>
     <t>IR/RH Configuration</t>
+  </si>
+  <si>
+    <t>QA Testing 091624/Cart 1 Outdoor Data/</t>
+  </si>
+  <si>
+    <t>QA Testing 091624/Cart 1 Indoor Data/</t>
+  </si>
+  <si>
+    <t>USB-TEMP (Device 0) - Analog - 9-16-2024 2-09-36.6 PM.csv</t>
+  </si>
+  <si>
+    <t>USB-TEMP (Device 0) - Analog - 9-16-2024 1-09-41.2 PM.csv</t>
+  </si>
+  <si>
+    <t>USB-1208FS-Plus (Device 1) - Analog - 9-16-2024 2-09-37.1 PM.csv</t>
+  </si>
+  <si>
+    <t>USB-1208FS-Plus (Device 1) - Analog - 9-16-2024 1-09-41.7 PM.csv</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Cart 1 Temp</t>
+  </si>
+  <si>
+    <t>Cart 1 IR</t>
+  </si>
+  <si>
+    <t>Cart 2 Temp</t>
+  </si>
+  <si>
+    <t>Cart 2 IR</t>
+  </si>
+  <si>
+    <t>QA Testing 091624/Cart 2 Indoor Data/</t>
+  </si>
+  <si>
+    <t>USB-TEMP (Device 0) - Analog - 9-16-2024 10-49-41.1 AM.csv</t>
+  </si>
+  <si>
+    <t>USB-1208FS-Plus (Device 1) - Analog - 9-16-2024 10-49-40.838 AM.csv</t>
+  </si>
+  <si>
+    <t>GPS Test</t>
+  </si>
+  <si>
+    <t>USB-TEMP (Device 1) - Analog - 8-9-2024 10-24-07.5 AM.csv</t>
+  </si>
+  <si>
+    <t>USB-1208FS-Plus (Device 0) - Analog - 8-9-2024 10-24-08.0 AM.csv</t>
+  </si>
+  <si>
+    <t>Midway080924east.csv</t>
+  </si>
+  <si>
+    <t>outdoor transect</t>
   </si>
 </sst>
 </file>
@@ -478,7 +508,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD5164DB-1ABC-4287-8BC5-0DED7AB536BB}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L5" sqref="L5"/>
@@ -496,37 +526,37 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" t="s">
+      <c r="K1" t="s">
         <v>13</v>
-      </c>
-      <c r="C1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -534,69 +564,139 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="F2" s="2">
         <v>45551</v>
       </c>
       <c r="G2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="F3" s="2">
         <v>45551</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
       <c r="I3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="2">
+        <v>45551</v>
+      </c>
+      <c r="G4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4">
         <v>2</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>7</v>
+      <c r="I4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="2">
+        <v>45513</v>
+      </c>
+      <c r="G5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>